<commit_message>
Add uplad question files and big refactor
</commit_message>
<xml_diff>
--- a/Interface web/uploads/exemple_liste.xlsx
+++ b/Interface web/uploads/exemple_liste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecambxl-my.sharepoint.com/personal/17076_ecam_be/Documents/Ecole/Master 1/Q2/Projet Robot/KorreKthor/Interface web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecambxl-my.sharepoint.com/personal/17076_ecam_be/Documents/Ecole/Master 1/Q2/Projet Robot/KorreKthor/Interface web/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_4086817CFE8FC2D621F05A6516DF56A869228FBC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8D320404-A15F-4F50-B824-257FB2DCFD79}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_4086817CFE8FC2D621F05A6516DF56A869228FBC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38B29996-C2DC-4EF9-A965-1918299A4BB7}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>cotes_2021_4eisd40_juin</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
 </sst>
 </file>
@@ -187,12 +184,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +473,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
@@ -492,16 +489,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -528,7 +525,7 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -549,7 +546,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -570,7 +567,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -591,7 +588,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -612,8 +609,8 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="8" t="s">
-        <v>33</v>
+      <c r="I6" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -633,8 +630,8 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="8" t="s">
-        <v>30</v>
+      <c r="I7" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -654,8 +651,8 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="8" t="s">
-        <v>31</v>
+      <c r="I8" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -675,8 +672,8 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="8" t="s">
-        <v>32</v>
+      <c r="I9" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -696,8 +693,8 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="8" t="s">
-        <v>33</v>
+      <c r="I10" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -717,8 +714,8 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="8" t="s">
-        <v>30</v>
+      <c r="I11" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -738,8 +735,8 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="8" t="s">
-        <v>31</v>
+      <c r="I12" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -759,8 +756,8 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="8" t="s">
-        <v>32</v>
+      <c r="I13" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -780,8 +777,8 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="8" t="s">
-        <v>33</v>
+      <c r="I14" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -801,7 +798,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -822,7 +819,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -840,7 +837,7 @@
       <c r="E17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -858,8 +855,8 @@
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>33</v>
+      <c r="I18" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
link uploaded files (questions) with the qcm gen
</commit_message>
<xml_diff>
--- a/Interface web/uploads/exemple_liste.xlsx
+++ b/Interface web/uploads/exemple_liste.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecambxl-my.sharepoint.com/personal/17076_ecam_be/Documents/Ecole/Master 1/Q2/Projet Robot/KorreKthor/Interface web/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecambxl-my.sharepoint.com/personal/17076_ecam_be/Documents/Ecole/Master 1/Q2/Projet Robot/KorreKthor/Interface web/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="11_4086817CFE8FC2D621F05A6516DF56A869228FBC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38B29996-C2DC-4EF9-A965-1918299A4BB7}"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
@@ -869,6 +869,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008363491AB45800439C60E5A4AFEEFD7B" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="bd968deeac1585f8dce456b69f03d27c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a086da1-f6b6-4775-9bed-6a1f1d23dd5e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03b8d306141823516372461e3a3187c9" ns2:_="">
     <xsd:import namespace="9a086da1-f6b6-4775-9bed-6a1f1d23dd5e"/>
@@ -1000,15 +1009,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1016,6 +1016,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB8E40AD-9265-40D6-9AF2-9D7659819022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC8E71B-4498-481C-B008-0BDAE5EBCBF4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1033,14 +1041,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB8E40AD-9265-40D6-9AF2-9D7659819022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0AB5F2-35DE-410C-B519-5BD2E467F978}">
   <ds:schemaRefs>

</xml_diff>